<commit_message>
[ANV] updated the xenon file
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/xenon.xlsx
+++ b/levelfiles/spreadsheet/xenon.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22F677A-EEBD-FF42-A773-4414F5BD0B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE1BEC7-3C52-754B-9C4C-4C500695DC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -89,7 +91,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269F673A-9A68-9948-B26F-F24DE369A567}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
@@ -423,7 +425,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -443,7 +445,7 @@
       <c r="A2">
         <v>131</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>99.65</v>
       </c>
       <c r="C2">
@@ -457,12 +459,15 @@
         <f>A2+1</f>
         <v>132</v>
       </c>
+      <c r="F2">
+        <v>6.604419</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>129</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>22.01</v>
       </c>
       <c r="C3">
@@ -473,15 +478,18 @@
         <v>581.07720600000005</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="0">A3+1</f>
+        <f>A3+1</f>
         <v>130</v>
+      </c>
+      <c r="F3">
+        <v>6.9068535000000004</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>130</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>4.8109999999999999</v>
       </c>
       <c r="C4">
@@ -492,114 +500,154 @@
         <v>19.585580999999998</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f>A4+1</f>
         <v>131</v>
+      </c>
+      <c r="F4">
+        <v>9.2557229999999997</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1">
-        <v>0.44500000000000001</v>
+        <v>148.4</v>
       </c>
       <c r="C5">
-        <v>26.9086</v>
+        <v>9.5200000000000007E-2</v>
       </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>11.974327000000001</v>
+        <v>14.127680000000002</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>133</v>
+        <f>A5+1</f>
+        <v>125</v>
+      </c>
+      <c r="F5">
+        <v>10.49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>128</v>
-      </c>
-      <c r="B6">
-        <v>5.2039999999999997</v>
+        <v>132</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.44500000000000001</v>
       </c>
       <c r="C6">
-        <v>1.9101999999999999</v>
+        <v>26.9086</v>
       </c>
       <c r="D6">
         <f>B6*C6</f>
-        <v>9.9406807999999991</v>
+        <v>11.974327000000001</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>129</v>
+        <f>A6+1</f>
+        <v>133</v>
+      </c>
+      <c r="F6">
+        <v>8.9367175999999997</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B7" s="1">
-        <v>0.26500000000000001</v>
+        <v>5.2039999999999997</v>
       </c>
       <c r="C7">
-        <v>10.435700000000001</v>
+        <v>1.9101999999999999</v>
       </c>
       <c r="D7">
         <f>B7*C7</f>
-        <v>2.7654605000000001</v>
+        <v>9.9406807999999991</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>135</v>
+        <f>A7+1</f>
+        <v>129</v>
+      </c>
+      <c r="F7">
+        <v>9.6110000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B8" s="1">
-        <v>0.13</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="C8">
-        <v>8.8573000000000004</v>
+        <v>10.435700000000001</v>
       </c>
       <c r="D8">
         <f>B8*C8</f>
-        <v>1.1514490000000002</v>
+        <v>2.7654605000000001</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>137</v>
+        <f>A8+1</f>
+        <v>135</v>
+      </c>
+      <c r="F8">
+        <v>8.5535999999999994</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>126</v>
-      </c>
-      <c r="B9">
-        <v>4.2720000000000002</v>
+        <v>136</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.13</v>
       </c>
       <c r="C9">
-        <v>8.8999999999999996E-2</v>
+        <v>8.8573000000000004</v>
       </c>
       <c r="D9">
         <f>B9*C9</f>
+        <v>1.1514490000000002</v>
+      </c>
+      <c r="E9">
+        <f>A9+1</f>
+        <v>137</v>
+      </c>
+      <c r="F9">
+        <v>8.0869999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>126</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.2720000000000002</v>
+      </c>
+      <c r="C10">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="D10">
+        <f>B10*C10</f>
         <v>0.38020799999999999</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
+      <c r="E10">
+        <f>A10+1</f>
         <v>127</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10">
-        <f>SUM(C2:C9)</f>
-        <v>99.904399999999995</v>
+      <c r="F10">
+        <v>10.0183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>SUM(C2:C10)</f>
+        <v>99.999599999999987</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
-    <sortCondition descending="1" ref="D2:D9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
+    <sortCondition descending="1" ref="D2:D10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[ANV] started on xenon gamma decays
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/xenon.xlsx
+++ b/levelfiles/spreadsheet/xenon.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE1BEC7-3C52-754B-9C4C-4C500695DC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C84329-5704-D448-9708-E2454FB931ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
+    <sheet name="132-primary gammas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>iso</t>
   </si>
@@ -54,6 +55,21 @@
   </si>
   <si>
     <t>Sn (MeV)</t>
+  </si>
+  <si>
+    <t>Gamma Energy (keV)</t>
+  </si>
+  <si>
+    <t>relative abundance</t>
+  </si>
+  <si>
+    <t>initial level (keV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference: https://iopscience.iop.org/article/10.1088/0305-4616/14/9/009 </t>
+  </si>
+  <si>
+    <t>Sn:</t>
   </si>
 </sst>
 </file>
@@ -408,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269F673A-9A68-9948-B26F-F24DE369A567}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,15 +468,15 @@
         <v>21.231999999999999</v>
       </c>
       <c r="D2">
-        <f>B2*C2</f>
+        <f t="shared" ref="D2:D10" si="0">B2*C2</f>
         <v>2115.7687999999998</v>
       </c>
       <c r="E2">
-        <f>A2+1</f>
+        <f t="shared" ref="E2:E10" si="1">A2+1</f>
         <v>132</v>
       </c>
       <c r="F2">
-        <v>6.604419</v>
+        <v>8.9367175999999997</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -474,15 +490,15 @@
         <v>26.400600000000001</v>
       </c>
       <c r="D3">
-        <f>B3*C3</f>
+        <f t="shared" si="0"/>
         <v>581.07720600000005</v>
       </c>
       <c r="E3">
-        <f>A3+1</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="F3">
-        <v>6.9068535000000004</v>
+        <v>9.2557229999999997</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -496,15 +512,15 @@
         <v>4.0709999999999997</v>
       </c>
       <c r="D4">
-        <f>B4*C4</f>
+        <f t="shared" si="0"/>
         <v>19.585580999999998</v>
       </c>
       <c r="E4">
-        <f>A4+1</f>
+        <f t="shared" si="1"/>
         <v>131</v>
       </c>
       <c r="F4">
-        <v>9.2557229999999997</v>
+        <v>6.604419</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -518,15 +534,15 @@
         <v>9.5200000000000007E-2</v>
       </c>
       <c r="D5">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>14.127680000000002</v>
       </c>
       <c r="E5">
-        <f>A5+1</f>
+        <f t="shared" si="1"/>
         <v>125</v>
       </c>
       <c r="F5">
-        <v>10.49</v>
+        <v>7.6032999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -540,15 +556,15 @@
         <v>26.9086</v>
       </c>
       <c r="D6">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>11.974327000000001</v>
       </c>
       <c r="E6">
-        <f>A6+1</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="F6">
-        <v>8.9367175999999997</v>
+        <v>6.4359000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -562,15 +578,15 @@
         <v>1.9101999999999999</v>
       </c>
       <c r="D7">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>9.9406807999999991</v>
       </c>
       <c r="E7">
-        <f>A7+1</f>
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
       <c r="F7">
-        <v>9.6110000000000007</v>
+        <v>6.9068535000000004</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -584,15 +600,15 @@
         <v>10.435700000000001</v>
       </c>
       <c r="D8">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>2.7654605000000001</v>
       </c>
       <c r="E8">
-        <f>A8+1</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="F8">
-        <v>8.5535999999999994</v>
+        <v>6.359</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -606,15 +622,15 @@
         <v>8.8573000000000004</v>
       </c>
       <c r="D9">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>1.1514490000000002</v>
       </c>
       <c r="E9">
-        <f>A9+1</f>
+        <f t="shared" si="1"/>
         <v>137</v>
       </c>
       <c r="F9">
-        <v>8.0869999999999997</v>
+        <v>4.0255599999999996</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -628,15 +644,15 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="D10">
-        <f>B10*C10</f>
+        <f t="shared" si="0"/>
         <v>0.38020799999999999</v>
       </c>
       <c r="E10">
-        <f>A10+1</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="F10">
-        <v>10.0183</v>
+        <v>7.2460000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -651,4 +667,74 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327F00C6-A195-6345-B007-0EDDFE20AB60}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <f>8.9367176*1000</f>
+        <v>8936.7175999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>$E$1-C3</f>
+        <v>5694.1175999999996</v>
+      </c>
+      <c r="C3">
+        <v>3242.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A5" si="0">$E$1-C4</f>
+        <v>5755.3176000000003</v>
+      </c>
+      <c r="C4">
+        <v>3181.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>6063.7175999999999</v>
+      </c>
+      <c r="C5">
+        <v>2873</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[ANV] added various gamma transitions
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/xenon.xlsx
+++ b/levelfiles/spreadsheet/xenon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C00B8-0578-454B-B720-5DD33582C1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07804B9F-29FC-F845-A145-3DDF89C2FF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
   <sheets>
     <sheet name="isotopes" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>Gamma Energy (keV)</t>
   </si>
   <si>
-    <t>relative abundance</t>
-  </si>
-  <si>
     <t>initial level (keV)</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Cap. Percent (%)</t>
+  </si>
+  <si>
+    <t>relative abundance (b)</t>
   </si>
 </sst>
 </file>
@@ -88,15 +88,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,13 +110,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269F673A-9A68-9948-B26F-F24DE369A567}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -461,7 +493,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,27 +750,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327F00C6-A195-6345-B007-0EDDFE20AB60}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <f>8.9367176*1000</f>
         <v>8936.7175999999999</v>
       </c>
@@ -748,37 +782,718 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <f>$E$1-C3</f>
-        <v>5694.1175999999996</v>
-      </c>
-      <c r="C3">
-        <v>3242.6</v>
+        <v>8936.7175999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f t="shared" ref="A4:A5" si="0">$E$1-C4</f>
-        <v>5755.3176000000003</v>
-      </c>
-      <c r="C4">
-        <v>3181.4</v>
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A67" si="0">$E$1-C4</f>
+        <v>8269.0025999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>667.71500000000003</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>6063.7175999999999</v>
-      </c>
-      <c r="C5">
-        <v>2873</v>
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>7638.8055999999997</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1297.912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>7496.3945999999996</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1440.3230000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>7133.0036</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1803.7139999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>7086.7175999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>6973.7075999999997</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1963.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>6951.0766000000003</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1985.6410000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>6896.4076000000005</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2040.31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>6826.4375999999993</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2110.2800000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>6824.8375999999998</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2111.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>6769.6275999999998</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2167.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>6767.9175999999998</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2168.8000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>6749.3176000000003</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2187.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>6722.7075999999997</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2214.0100000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>6633.2975999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2303.42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>6586.0776000000005</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2350.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>6583.6175999999996</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2353.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>6541.7975999999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2394.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>6511.9475999999995</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2424.77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <f t="shared" si="0"/>
+        <v>6467.9375999999993</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1.33</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2468.7800000000002</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>6446.7175999999999</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2490</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>6424.5176000000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2512.1999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <f t="shared" si="0"/>
+        <v>6381.1075999999994</v>
+      </c>
+      <c r="B26" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="C26" s="6">
+        <v>2555.61</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>6352.9475999999995</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2583.77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>6348.0275999999994</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2588.69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>6323.2676000000001</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2613.4499999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>6286.4175999999998</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2650.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>6266.7276000000002</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2669.99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>6222.3176000000003</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2714.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>6184.5075999999999</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2752.21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>6182.2875999999997</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2754.43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>6108.7175999999999</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2828</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
+        <v>6097.8675999999996</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2838.85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>6096.6175999999996</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2840.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>6064.0176000000001</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2872.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>6046.0275999999994</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2890.69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>6019.8675999999996</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2916.85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
+        <v>6001.5176000000001</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2935.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>5977.9575999999997</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2958.76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>5976.4175999999998</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2960.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>5887.1175999999996</v>
+      </c>
+      <c r="C44" s="2">
+        <v>3049.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>5878.5776000000005</v>
+      </c>
+      <c r="C45" s="2">
+        <v>3058.14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
+        <v>5860.2875999999997</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3076.43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>5852.3176000000003</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3084.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>5824.6376</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3112.08</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>5814.7875999999997</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3121.93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>5781.0576000000001</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3155.66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
+        <v>5756.0176000000001</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3180.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <f t="shared" si="0"/>
+        <v>5743.9076000000005</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3192.81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <f t="shared" si="0"/>
+        <v>5722.7476000000006</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3213.97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <f t="shared" si="0"/>
+        <v>5710.0075999999999</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3226.71</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <f t="shared" si="0"/>
+        <v>5699.5176000000001</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3237.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <f t="shared" si="0"/>
+        <v>5693.3176000000003</v>
+      </c>
+      <c r="C56" s="2">
+        <v>3243.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <f t="shared" si="0"/>
+        <v>5687.7175999999999</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <f t="shared" si="0"/>
+        <v>5675.8176000000003</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3260.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <f t="shared" si="0"/>
+        <v>5616.3176000000003</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3320.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <f t="shared" si="0"/>
+        <v>5583.4175999999998</v>
+      </c>
+      <c r="C60" s="2">
+        <v>3353.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <f t="shared" si="0"/>
+        <v>5551.5176000000001</v>
+      </c>
+      <c r="C61" s="2">
+        <v>3385.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <f t="shared" si="0"/>
+        <v>5237.2175999999999</v>
+      </c>
+      <c r="C62" s="3">
+        <v>3699.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <f t="shared" si="0"/>
+        <v>5203.7175999999999</v>
+      </c>
+      <c r="C63" s="2">
+        <v>3733</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <f t="shared" si="0"/>
+        <v>5144.2175999999999</v>
+      </c>
+      <c r="C64" s="3">
+        <v>3792.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <f t="shared" si="0"/>
+        <v>5111.7175999999999</v>
+      </c>
+      <c r="C65" s="2">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <f t="shared" si="0"/>
+        <v>5081.7175999999999</v>
+      </c>
+      <c r="C66" s="2">
+        <v>3855</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <f t="shared" si="0"/>
+        <v>5061.4175999999998</v>
+      </c>
+      <c r="C67" s="3">
+        <v>3875.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <f t="shared" ref="A68:A79" si="1">$E$1-C68</f>
+        <v>5027.7175999999999</v>
+      </c>
+      <c r="C68" s="2">
+        <v>3909</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <f t="shared" si="1"/>
+        <v>4982.5176000000001</v>
+      </c>
+      <c r="C69" s="3">
+        <v>3954.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <f t="shared" si="1"/>
+        <v>4946.7175999999999</v>
+      </c>
+      <c r="C70" s="2">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <f t="shared" si="1"/>
+        <v>4918.7175999999999</v>
+      </c>
+      <c r="C71" s="2">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <f t="shared" si="1"/>
+        <v>4909.7175999999999</v>
+      </c>
+      <c r="C72" s="3">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <f t="shared" si="1"/>
+        <v>4842.2175999999999</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0.107</v>
+      </c>
+      <c r="C73" s="6">
+        <v>4094.5</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <f t="shared" si="1"/>
+        <v>4826.7175999999999</v>
+      </c>
+      <c r="C74" s="2">
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <f t="shared" si="1"/>
+        <v>4789.7175999999999</v>
+      </c>
+      <c r="C75" s="2">
+        <v>4147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <f t="shared" si="1"/>
+        <v>4768.7175999999999</v>
+      </c>
+      <c r="C76" s="2">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <f t="shared" si="1"/>
+        <v>4748.3176000000003</v>
+      </c>
+      <c r="C77" s="2">
+        <v>4188.3999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <f t="shared" si="1"/>
+        <v>4736.7175999999999</v>
+      </c>
+      <c r="C78" s="2">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f t="shared" si="1"/>
+        <v>4706.7175999999999</v>
+      </c>
+      <c r="C79" s="2">
+        <v>4230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>